<commit_message>
More benchmark datat into the system
</commit_message>
<xml_diff>
--- a/bench/malte.xlsx
+++ b/bench/malte.xlsx
@@ -451,9 +451,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4572A7"/>
-            </a:solidFill>
+            <a:pattFill prst="pct5">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="tx2"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -461,23 +466,59 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+              <c:f>Sheet4!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>ContextL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ContextJS Edge</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ContextJS Chrome OSX</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ContextJS Chrome Win</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ContextPy Python OSX</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ContextPy PyPy OSX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$2</c:f>
+              <c:f>Sheet4!$B$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.671715222843913</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000412458193122127</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00133243676817078</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000547716181384589</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0408880651880897</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.042993344126641</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.189976252968379</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -498,9 +539,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="AA4643"/>
-            </a:solidFill>
+            <a:pattFill prst="pct50">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -508,23 +554,59 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+              <c:f>Sheet4!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>ContextL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ContextJS Edge</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ContextJS Chrome OSX</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ContextJS Chrome Win</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ContextPy Python OSX</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ContextPy PyPy OSX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$3</c:f>
+              <c:f>Sheet4!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.358972593306707</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000940233236151603</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000932570573538186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000306217387968078</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0406786663792484</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.841919972522754</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.601038961038961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -545,9 +627,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="89A54E"/>
-            </a:solidFill>
+            <a:pattFill prst="ltDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent3"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -555,23 +642,59 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+              <c:f>Sheet4!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>ContextL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ContextJS Edge</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ContextJS Chrome OSX</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ContextJS Chrome Win</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ContextPy Python OSX</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ContextPy PyPy OSX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$4</c:f>
+              <c:f>Sheet4!$B$4:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.366578977467688</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000812523381967826</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000739166091160221</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000260445957683463</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0381462559097148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.510296136497352</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.182041066503217</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -592,9 +715,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="71588F"/>
-            </a:solidFill>
+            <a:pattFill prst="ltVert">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent4"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -602,23 +730,59 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+              <c:f>Sheet4!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>ContextL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ContextJS Edge</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ContextJS Chrome OSX</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ContextJS Chrome Win</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ContextPy Python OSX</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ContextPy PyPy OSX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$5</c:f>
+              <c:f>Sheet4!$B$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.437545845122079</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000981984082234559</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000630244136676102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000208129080773653</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0378660216887056</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.395482845409988</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.024945950440712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -639,9 +803,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4198AF"/>
-            </a:solidFill>
+            <a:pattFill prst="dashDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:srgbClr val="4198AF"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -649,23 +818,59 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+              <c:f>Sheet4!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>ContextL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ContextJS Edge</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ContextJS Chrome OSX</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ContextJS Chrome Win</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ContextPy Python OSX</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ContextPy PyPy OSX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$6</c:f>
+              <c:f>Sheet4!$B$6:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.449037423533645</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000811567618954758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000547594500466309</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000441011229189147</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0360283756863126</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.277562373567094</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.902904787520172</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -686,33 +891,71 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="DB843D"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="zigZag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent6"/>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+              <c:f>Sheet4!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>ContextL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ContextJS Edge</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ContextJS Chrome OSX</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ContextJS Chrome Win</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ContextPy Python OSX</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ContextPy PyPy OSX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$7</c:f>
+              <c:f>Sheet4!$B$7:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.478076492238758</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00124868357428534</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000515129342900302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000454510615258836</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0353800330641746</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.294604371921182</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.945786826934871</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -733,33 +976,74 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="93A9CF"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="divot">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+              <c:f>Sheet4!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>ContextL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ContextJS Edge</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ContextJS Chrome OSX</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ContextJS Chrome Win</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ContextPy Python OSX</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ContextPy PyPy OSX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$8</c:f>
+              <c:f>Sheet4!$B$8:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.779464931308749</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00219063805122221</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000549703054298642</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000539118812376787</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0358148486972638</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.269481778237271</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.832150821001419</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -780,33 +1064,74 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="D19392"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="smGrid">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+              <c:f>Sheet4!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>ContextL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ContextJS Edge</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ContextJS Chrome OSX</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ContextJS Chrome Win</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ContextPy Python OSX</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ContextPy PyPy OSX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$9</c:f>
+              <c:f>Sheet4!$B$9:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.42771855010661</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00183284921576571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000557055504493464</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000506861863938053</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0342998843472915</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.120892139693005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.168771282633371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -827,33 +1152,74 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="B9CD96"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="pct10">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+              <c:f>Sheet4!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>ContextL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ContextJS Edge</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ContextJS Chrome OSX</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ContextJS Chrome Win</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ContextPy Python OSX</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ContextPy PyPy OSX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$10</c:f>
+              <c:f>Sheet4!$B$10:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.498718975180144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00178874600910709</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000599825075642965</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000546189101180195</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0339139392236737</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0550017262213016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0555808212058212</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -874,33 +1240,74 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="A99BBD"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="pct60">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+              <c:f>Sheet4!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>ContextL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ContextJS Edge</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ContextJS Chrome OSX</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ContextJS Chrome Win</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ContextPy Python OSX</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ContextPy PyPy OSX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$11</c:f>
+              <c:f>Sheet4!$B$11:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.3789957134109</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00177534818194815</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000595634815183102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000618550145348837</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0336262561292424</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0464943244739756</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0479021103664623</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -915,11 +1322,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2085652344"/>
-        <c:axId val="2085648632"/>
+        <c:axId val="-2120837848"/>
+        <c:axId val="-2134682072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2085652344"/>
+        <c:axId val="-2120837848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +1344,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2085648632"/>
+        <c:crossAx val="-2134682072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -945,10 +1352,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2085648632"/>
+        <c:axId val="-2134682072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.9"/>
+          <c:max val="4.2"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -974,7 +1382,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2085652344"/>
+        <c:crossAx val="-2120837848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -992,9 +1400,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525">
       <a:noFill/>
     </a:ln>
@@ -1004,8 +1410,8 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1000">
-          <a:latin typeface="Source Sans Pro"/>
+        <a:defRPr sz="1000" kern="100">
+          <a:latin typeface="Times New Roman"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -1055,9 +1461,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4572A7"/>
-            </a:solidFill>
+            <a:pattFill prst="pct5">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="tx2"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -1065,29 +1476,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$G$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ContextPyPy PyPy OSX</c:v>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ContextL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$G$2:$H$2</c:f>
+              <c:f>Sheet4!$B$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>3.042993344126641</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.189976252968379</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.671715222843913</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1108,9 +1513,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="AA4643"/>
-            </a:solidFill>
+            <a:pattFill prst="pct50">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -1118,29 +1528,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$G$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ContextPyPy PyPy OSX</c:v>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ContextL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$G$3:$H$3</c:f>
+              <c:f>Sheet4!$B$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.841919972522754</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.601038961038961</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.358972593306707</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1161,9 +1565,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="89A54E"/>
-            </a:solidFill>
+            <a:pattFill prst="ltDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent3"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -1171,29 +1580,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$G$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ContextPyPy PyPy OSX</c:v>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ContextL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$G$4:$H$4</c:f>
+              <c:f>Sheet4!$B$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.510296136497352</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.182041066503217</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.366578977467688</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1214,9 +1617,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="71588F"/>
-            </a:solidFill>
+            <a:pattFill prst="ltVert">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent4"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -1224,29 +1632,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$G$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ContextPyPy PyPy OSX</c:v>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ContextL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$G$5:$H$5</c:f>
+              <c:f>Sheet4!$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.395482845409988</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.024945950440712</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.437545845122079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1267,9 +1669,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4198AF"/>
-            </a:solidFill>
+            <a:pattFill prst="dashDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:srgbClr val="4198AF"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -1277,29 +1684,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$G$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ContextPyPy PyPy OSX</c:v>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ContextL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$G$6:$H$6</c:f>
+              <c:f>Sheet4!$B$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.277562373567094</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.902904787520172</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.449037423533645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1320,39 +1721,35 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="DB843D"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="zigZag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent6"/>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$G$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ContextPyPy PyPy OSX</c:v>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ContextL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$G$7:$H$7</c:f>
+              <c:f>Sheet4!$B$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.294604371921182</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.945786826934871</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.478076492238758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1373,39 +1770,38 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="93A9CF"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="divot">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$G$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ContextPyPy PyPy OSX</c:v>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ContextL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$G$8:$H$8</c:f>
+              <c:f>Sheet4!$B$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.269481778237271</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.832150821001419</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.779464931308749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1426,39 +1822,38 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="D19392"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="smGrid">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$G$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ContextPyPy PyPy OSX</c:v>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ContextL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$G$9:$H$9</c:f>
+              <c:f>Sheet4!$B$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.120892139693005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.168771282633371</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.42771855010661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1479,39 +1874,38 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="B9CD96"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="pct10">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$G$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ContextPyPy PyPy OSX</c:v>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ContextL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$G$10:$H$10</c:f>
+              <c:f>Sheet4!$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.0550017262213016</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0555808212058212</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.498718975180144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1532,39 +1926,38 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="A99BBD"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="pct60">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$G$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ContextPyPy PyPy OSX</c:v>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ContextL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$G$11:$H$11</c:f>
+              <c:f>Sheet4!$B$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.0464943244739756</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0479021103664623</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.3789957134109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1579,11 +1972,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2140431032"/>
-        <c:axId val="2140427368"/>
+        <c:axId val="-2079237624"/>
+        <c:axId val="-2079241224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2140431032"/>
+        <c:axId val="-2079237624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1601,7 +1994,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2140427368"/>
+        <c:crossAx val="-2079241224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1609,10 +2002,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140427368"/>
+        <c:axId val="-2079241224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4.5"/>
+          <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1638,7 +2031,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2140431032"/>
+        <c:crossAx val="-2079237624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1656,9 +2049,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525">
       <a:noFill/>
     </a:ln>
@@ -1668,8 +2059,8 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1000">
-          <a:latin typeface="Source Sans Pro"/>
+        <a:defRPr sz="1000" kern="100">
+          <a:latin typeface="Times New Roman"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -1719,9 +2110,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4572A7"/>
-            </a:solidFill>
+            <a:pattFill prst="pct5">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="tx2"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -1784,9 +2180,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="AA4643"/>
-            </a:solidFill>
+            <a:pattFill prst="pct50">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -1849,9 +2250,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="89A54E"/>
-            </a:solidFill>
+            <a:pattFill prst="ltDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent3"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -1914,9 +2320,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="71588F"/>
-            </a:solidFill>
+            <a:pattFill prst="ltVert">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent4"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -1979,9 +2390,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4198AF"/>
-            </a:solidFill>
+            <a:pattFill prst="dashDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:srgbClr val="4198AF"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="25400">
               <a:noFill/>
             </a:ln>
@@ -2044,12 +2460,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="DB843D"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="zigZag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent6"/>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -2109,12 +2527,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="93A9CF"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="divot">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -2174,12 +2597,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="D19392"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="smGrid">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -2239,12 +2667,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="B9CD96"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
+            <a:pattFill prst="pct10">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -2303,6 +2736,19 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct60">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2355,11 +2801,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2140367992"/>
-        <c:axId val="2140364344"/>
+        <c:axId val="-2078484056"/>
+        <c:axId val="-2078498328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2140367992"/>
+        <c:axId val="-2078484056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2377,7 +2823,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2140364344"/>
+        <c:crossAx val="-2078498328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2385,9 +2831,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140364344"/>
+        <c:axId val="-2078498328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.042"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2413,9 +2861,10 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2140367992"/>
+        <c:crossAx val="-2078484056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:minorUnit val="0.001"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -2431,9 +2880,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525">
       <a:noFill/>
     </a:ln>
@@ -2443,8 +2890,8 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1000">
-          <a:latin typeface="Source Sans Pro"/>
+        <a:defRPr sz="1000" kern="100">
+          <a:latin typeface="Times New Roman"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -2509,28 +2956,13 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ContextL</c:v>
+              <c:f>Sheet4!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ContextPy PyPy OSX</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ContextJS Edge</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ContextJS Chrome OSX</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ContextJS Chrome Win</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>ContextPy Python OSX</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
@@ -2538,29 +2970,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$2:$H$2</c:f>
+              <c:f>Sheet4!$G$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.671715222843913</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.042993344126641</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000412458193122127</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.00133243676817078</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000547716181384589</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0408880651880897</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.042993344126641</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>4.189976252968379</c:v>
                 </c:pt>
               </c:numCache>
@@ -2597,28 +3014,13 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ContextL</c:v>
+              <c:f>Sheet4!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ContextPy PyPy OSX</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ContextJS Edge</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ContextJS Chrome OSX</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ContextJS Chrome Win</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>ContextPy Python OSX</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
@@ -2626,29 +3028,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$3:$H$3</c:f>
+              <c:f>Sheet4!$G$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.358972593306707</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.841919972522754</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000940233236151603</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.000932570573538186</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000306217387968078</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0406786663792484</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.841919972522754</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>2.601038961038961</c:v>
                 </c:pt>
               </c:numCache>
@@ -2685,28 +3072,13 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ContextL</c:v>
+              <c:f>Sheet4!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ContextPy PyPy OSX</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ContextJS Edge</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ContextJS Chrome OSX</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ContextJS Chrome Win</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>ContextPy Python OSX</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
@@ -2714,29 +3086,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$4:$H$4</c:f>
+              <c:f>Sheet4!$G$4:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.366578977467688</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.510296136497352</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000812523381967826</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.000739166091160221</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000260445957683463</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0381462559097148</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.510296136497352</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>2.182041066503217</c:v>
                 </c:pt>
               </c:numCache>
@@ -2773,28 +3130,13 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ContextL</c:v>
+              <c:f>Sheet4!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ContextPy PyPy OSX</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ContextJS Edge</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ContextJS Chrome OSX</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ContextJS Chrome Win</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>ContextPy Python OSX</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
@@ -2802,29 +3144,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$5:$H$5</c:f>
+              <c:f>Sheet4!$G$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.437545845122079</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.395482845409988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000981984082234559</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.000630244136676102</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000208129080773653</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0378660216887056</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.395482845409988</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>2.024945950440712</c:v>
                 </c:pt>
               </c:numCache>
@@ -2861,28 +3188,13 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ContextL</c:v>
+              <c:f>Sheet4!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ContextPy PyPy OSX</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ContextJS Edge</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ContextJS Chrome OSX</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ContextJS Chrome Win</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>ContextPy Python OSX</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
@@ -2890,29 +3202,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$6:$H$6</c:f>
+              <c:f>Sheet4!$G$6:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.449037423533645</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.277562373567094</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000811567618954758</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.000547594500466309</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000441011229189147</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0360283756863126</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.277562373567094</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.902904787520172</c:v>
                 </c:pt>
               </c:numCache>
@@ -2946,28 +3243,13 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ContextL</c:v>
+              <c:f>Sheet4!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ContextPy PyPy OSX</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ContextJS Edge</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ContextJS Chrome OSX</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ContextJS Chrome Win</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>ContextPy Python OSX</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
@@ -2975,29 +3257,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$7:$H$7</c:f>
+              <c:f>Sheet4!$G$7:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.478076492238758</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.294604371921182</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00124868357428534</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.000515129342900302</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000454510615258836</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0353800330641746</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.294604371921182</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.945786826934871</c:v>
                 </c:pt>
               </c:numCache>
@@ -3034,28 +3301,13 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ContextL</c:v>
+              <c:f>Sheet4!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ContextPy PyPy OSX</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ContextJS Edge</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ContextJS Chrome OSX</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ContextJS Chrome Win</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>ContextPy Python OSX</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
@@ -3063,29 +3315,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$8:$H$8</c:f>
+              <c:f>Sheet4!$G$8:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.779464931308749</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.269481778237271</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00219063805122221</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.000549703054298642</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000539118812376787</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0358148486972638</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.269481778237271</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.832150821001419</c:v>
                 </c:pt>
               </c:numCache>
@@ -3122,28 +3359,13 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ContextL</c:v>
+              <c:f>Sheet4!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ContextPy PyPy OSX</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ContextJS Edge</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ContextJS Chrome OSX</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ContextJS Chrome Win</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>ContextPy Python OSX</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
@@ -3151,29 +3373,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$9:$H$9</c:f>
+              <c:f>Sheet4!$G$9:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.42771855010661</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.120892139693005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00183284921576571</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.000557055504493464</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000506861863938053</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0342998843472915</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.120892139693005</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.168771282633371</c:v>
                 </c:pt>
               </c:numCache>
@@ -3210,28 +3417,13 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ContextL</c:v>
+              <c:f>Sheet4!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ContextPy PyPy OSX</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ContextJS Edge</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ContextJS Chrome OSX</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ContextJS Chrome Win</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>ContextPy Python OSX</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
@@ -3239,29 +3431,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$10:$H$10</c:f>
+              <c:f>Sheet4!$G$10:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.498718975180144</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.0550017262213016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00178874600910709</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.000599825075642965</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000546189101180195</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0339139392236737</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0550017262213016</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.0555808212058212</c:v>
                 </c:pt>
               </c:numCache>
@@ -3298,28 +3475,13 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>ContextL</c:v>
+              <c:f>Sheet4!$G$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ContextPy PyPy OSX</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ContextJS Edge</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ContextJS Chrome OSX</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ContextJS Chrome Win</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>ContextPy Python OSX</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ContextPy PyPy OSX</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>ContextPyPy PyPy OSX</c:v>
                 </c:pt>
               </c:strCache>
@@ -3327,29 +3489,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$11:$H$11</c:f>
+              <c:f>Sheet4!$G$11:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.3789957134109</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.0464943244739756</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00177534818194815</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.000595634815183102</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000618550145348837</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0336262561292424</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0464943244739756</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.0479021103664623</c:v>
                 </c:pt>
               </c:numCache>
@@ -3365,11 +3512,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2127600904"/>
-        <c:axId val="-2127585400"/>
+        <c:axId val="-2133424088"/>
+        <c:axId val="-2079446808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2127600904"/>
+        <c:axId val="-2133424088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3387,7 +3534,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2127585400"/>
+        <c:crossAx val="-2079446808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3395,10 +3542,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2127585400"/>
+        <c:axId val="-2079446808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
+          <c:max val="4.3"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3424,7 +3572,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2127600904"/>
+        <c:crossAx val="-2133424088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4046,17 +4194,17 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1574800</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2197100</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 4"/>
+        <xdr:cNvPr id="9" name="Chart 8"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4075,20 +4223,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1511300</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 4"/>
+        <xdr:cNvPr id="10" name="Chart 9"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4107,20 +4255,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1778000</xdr:colOff>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 4"/>
+        <xdr:cNvPr id="11" name="Chart 10"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4140,19 +4288,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="12" name="Chart 11"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -6716,8 +6864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
More benches, and plus purple
</commit_message>
<xml_diff>
--- a/bench/malte.xlsx
+++ b/bench/malte.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="50420" yWindow="7280" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="35440" yWindow="900" windowWidth="40580" windowHeight="22440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Bench1" sheetId="1" r:id="rId1"/>
@@ -512,13 +512,13 @@
                   <c:v>0.000547716181384589</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.039091651119403</c:v>
+                  <c:v>0.0420141213707469</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.008945798982634</c:v>
+                  <c:v>3.473300450353849</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.448480262328162</c:v>
+                  <c:v>4.417305443679356</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -600,13 +600,13 @@
                   <c:v>0.000306217387968078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0393120712355346</c:v>
+                  <c:v>0.0411001012584985</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.803968384653384</c:v>
+                  <c:v>0.727575805683442</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.569042025580788</c:v>
+                  <c:v>2.438208310847274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -688,13 +688,13 @@
                   <c:v>0.000260445957683463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0369627789121503</c:v>
+                  <c:v>0.0385837406740417</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.499716016660356</c:v>
+                  <c:v>0.47069092245498</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.990243902439024</c:v>
+                  <c:v>2.441516412390199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -776,13 +776,13 @@
                   <c:v>0.000208129080773653</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0361570840906917</c:v>
+                  <c:v>0.0379666079800597</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.407708306252437</c:v>
+                  <c:v>0.374806501547988</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.068036154478225</c:v>
+                  <c:v>1.969235913726801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -864,13 +864,13 @@
                   <c:v>0.000441011229189147</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0350284828946133</c:v>
+                  <c:v>0.0365167631179076</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.27175697865353</c:v>
+                  <c:v>0.278977560317192</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.866287528104748</c:v>
+                  <c:v>0.866490066225165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -949,13 +949,13 @@
                   <c:v>0.000454510615258836</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0358034970857619</c:v>
+                  <c:v>0.0357599847540225</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.274138664398128</c:v>
+                  <c:v>0.286732373009856</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.954928588152657</c:v>
+                  <c:v>0.944204419207505</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1037,13 +1037,13 @@
                   <c:v>0.000539118812376787</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0351666744697785</c:v>
+                  <c:v>0.0345276137754072</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.264704053717981</c:v>
+                  <c:v>0.264049219840162</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.861472742066721</c:v>
+                  <c:v>0.901389324140813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1125,13 +1125,13 @@
                   <c:v>0.000506861863938053</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0350124110201653</c:v>
+                  <c:v>0.0342104989766978</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.114233141038393</c:v>
+                  <c:v>0.123750650702759</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.160436623629043</c:v>
+                  <c:v>0.160632028180463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1213,13 +1213,13 @@
                   <c:v>0.000546189101180195</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0335966430255808</c:v>
+                  <c:v>0.0343119865571322</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0532972928359194</c:v>
+                  <c:v>0.051672171758877</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0554045376712329</c:v>
+                  <c:v>0.0534722222222222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1301,13 +1301,13 @@
                   <c:v>0.000618550145348837</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0340827951056441</c:v>
+                  <c:v>0.0349619251717391</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0466963916815865</c:v>
+                  <c:v>0.0441571580204325</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.04722718526663</c:v>
+                  <c:v>0.0450537315400844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1322,11 +1322,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2121668328"/>
-        <c:axId val="2121671624"/>
+        <c:axId val="-2119908040"/>
+        <c:axId val="-2119904760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121668328"/>
+        <c:axId val="-2119908040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,7 +1344,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2121671624"/>
+        <c:crossAx val="-2119904760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1352,7 +1352,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121671624"/>
+        <c:axId val="-2119904760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.2"/>
@@ -1382,7 +1382,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2121668328"/>
+        <c:crossAx val="-2119908040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1972,11 +1972,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2121758376"/>
-        <c:axId val="2121761528"/>
+        <c:axId val="2079582776"/>
+        <c:axId val="2079450088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121758376"/>
+        <c:axId val="2079582776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1994,7 +1994,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2121761528"/>
+        <c:crossAx val="2079450088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2002,7 +2002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121761528"/>
+        <c:axId val="2079450088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2031,7 +2031,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2121758376"/>
+        <c:crossAx val="2079582776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2159,7 +2159,7 @@
                   <c:v>0.000547716181384589</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.039091651119403</c:v>
+                  <c:v>0.0420141213707469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2229,7 +2229,7 @@
                   <c:v>0.000306217387968078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0393120712355346</c:v>
+                  <c:v>0.0411001012584985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2299,7 +2299,7 @@
                   <c:v>0.000260445957683463</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0369627789121503</c:v>
+                  <c:v>0.0385837406740417</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2369,7 +2369,7 @@
                   <c:v>0.000208129080773653</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0361570840906917</c:v>
+                  <c:v>0.0379666079800597</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2439,7 +2439,7 @@
                   <c:v>0.000441011229189147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0350284828946133</c:v>
+                  <c:v>0.0365167631179076</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2506,7 +2506,7 @@
                   <c:v>0.000454510615258836</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0358034970857619</c:v>
+                  <c:v>0.0357599847540225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2576,7 +2576,7 @@
                   <c:v>0.000539118812376787</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0351666744697785</c:v>
+                  <c:v>0.0345276137754072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2646,7 +2646,7 @@
                   <c:v>0.000506861863938053</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0350124110201653</c:v>
+                  <c:v>0.0342104989766978</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2716,7 +2716,7 @@
                   <c:v>0.000546189101180195</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0335966430255808</c:v>
+                  <c:v>0.0343119865571322</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2786,7 +2786,7 @@
                   <c:v>0.000618550145348837</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0340827951056441</c:v>
+                  <c:v>0.0349619251717391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2801,11 +2801,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2121825480"/>
-        <c:axId val="2121828584"/>
+        <c:axId val="-2121223880"/>
+        <c:axId val="-2129376424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121825480"/>
+        <c:axId val="-2121223880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2823,7 +2823,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2121828584"/>
+        <c:crossAx val="-2129376424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2831,7 +2831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121828584"/>
+        <c:axId val="-2129376424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.042"/>
@@ -2861,7 +2861,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2121825480"/>
+        <c:crossAx val="-2121223880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.001"/>
@@ -2975,10 +2975,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3.008945798982634</c:v>
+                  <c:v>3.473300450353849</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.448480262328162</c:v>
+                  <c:v>4.417305443679356</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3033,10 +3033,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.803968384653384</c:v>
+                  <c:v>0.727575805683442</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.569042025580788</c:v>
+                  <c:v>2.438208310847274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3091,10 +3091,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.499716016660356</c:v>
+                  <c:v>0.47069092245498</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.990243902439024</c:v>
+                  <c:v>2.441516412390199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3149,10 +3149,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.407708306252437</c:v>
+                  <c:v>0.374806501547988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.068036154478225</c:v>
+                  <c:v>1.969235913726801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3207,10 +3207,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.27175697865353</c:v>
+                  <c:v>0.278977560317192</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.866287528104748</c:v>
+                  <c:v>0.866490066225165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3262,10 +3262,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.274138664398128</c:v>
+                  <c:v>0.286732373009856</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.954928588152657</c:v>
+                  <c:v>0.944204419207505</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3320,10 +3320,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.264704053717981</c:v>
+                  <c:v>0.264049219840162</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.861472742066721</c:v>
+                  <c:v>0.901389324140813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3378,10 +3378,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.114233141038393</c:v>
+                  <c:v>0.123750650702759</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.160436623629043</c:v>
+                  <c:v>0.160632028180463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3436,10 +3436,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.0532972928359194</c:v>
+                  <c:v>0.051672171758877</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0554045376712329</c:v>
+                  <c:v>0.0534722222222222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3494,10 +3494,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.0466963916815865</c:v>
+                  <c:v>0.0441571580204325</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.04722718526663</c:v>
+                  <c:v>0.0450537315400844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3512,11 +3512,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2121891496"/>
-        <c:axId val="2121894600"/>
+        <c:axId val="-2121120408"/>
+        <c:axId val="-2121180248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121891496"/>
+        <c:axId val="-2121120408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3534,7 +3534,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2121894600"/>
+        <c:crossAx val="-2121180248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3542,7 +3542,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121894600"/>
+        <c:axId val="-2121180248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.3"/>
@@ -3572,7 +3572,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2121891496"/>
+        <c:crossAx val="-2121120408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3712,13 +3712,13 @@
                   <c:v>0.711285876439111</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.868135174987211</c:v>
+                  <c:v>0.892232286233063</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.054254982600443</c:v>
+                  <c:v>0.895926299121923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.854427645788337</c:v>
+                  <c:v>0.801558073654391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3800,13 +3800,13 @@
                   <c:v>0.52009722551577</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.795651574350724</c:v>
+                  <c:v>0.804084219287957</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.687325977106321</c:v>
+                  <c:v>0.613685663577204</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.296373988612526</c:v>
+                  <c:v>0.218832173240526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3888,13 +3888,13 @@
                   <c:v>0.38593172620095</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.729179128998829</c:v>
+                  <c:v>0.722280752434196</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.501429431236834</c:v>
+                  <c:v>0.438433361510285</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.192225461613217</c:v>
+                  <c:v>0.13811871522015</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3976,13 +3976,13 @@
                   <c:v>0.29404075613353</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.663383488038754</c:v>
+                  <c:v>0.665083711469254</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.385929357266937</c:v>
+                  <c:v>0.347942754919499</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.145035929021851</c:v>
+                  <c:v>0.10319110138585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4064,13 +4064,13 @@
                   <c:v>0.227444778595873</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.61857283760024</c:v>
+                  <c:v>0.615941398947963</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.305397727272727</c:v>
+                  <c:v>0.301901435778036</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.11296402055968</c:v>
+                  <c:v>0.0808428571428571</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4085,11 +4085,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2118182392"/>
-        <c:axId val="2118178616"/>
+        <c:axId val="-2119206296"/>
+        <c:axId val="-2119210840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2118182392"/>
+        <c:axId val="-2119206296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4107,7 +4107,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2118178616"/>
+        <c:crossAx val="-2119210840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4115,7 +4115,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118178616"/>
+        <c:axId val="-2119210840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4144,7 +4144,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2118182392"/>
+        <c:crossAx val="-2119206296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4681,11 +4681,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S26" sqref="S26"/>
+      <selection pane="bottomRight" activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -4867,31 +4867,31 @@
         <v>25600000</v>
       </c>
       <c r="O3" s="8">
-        <v>5.3639999999999999</v>
+        <v>5.5220000000000002</v>
       </c>
       <c r="P3" s="10">
         <f>N3/O3</f>
-        <v>4772557.7926920205</v>
+        <v>4636001.4487504521</v>
       </c>
       <c r="Q3" s="5">
         <v>819200000</v>
       </c>
       <c r="R3" s="8">
-        <v>8.577</v>
+        <v>8.0980000000000008</v>
       </c>
       <c r="S3" s="10">
         <f>Q3/R3</f>
-        <v>95511251.020170227</v>
+        <v>101160780.43961471</v>
       </c>
       <c r="T3" s="5">
         <v>819200000</v>
       </c>
       <c r="U3" s="8">
-        <v>8.8179999999999996</v>
+        <v>8.5</v>
       </c>
       <c r="V3" s="10">
         <f>T3/U3</f>
-        <v>92900884.554320708</v>
+        <v>96376470.588235289</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -4942,31 +4942,31 @@
         <v>25600000</v>
       </c>
       <c r="O4" s="8">
-        <v>9.077</v>
+        <v>9.0920000000000005</v>
       </c>
       <c r="P4" s="10">
         <f t="shared" ref="P4:P12" si="4">N4/O4</f>
-        <v>2820315.0820755758</v>
+        <v>2815662.1205455344</v>
       </c>
       <c r="Q4" s="5">
         <v>819200000</v>
       </c>
       <c r="R4" s="8">
-        <v>9.7650000000000006</v>
+        <v>9.1660000000000004</v>
       </c>
       <c r="S4" s="10">
         <f t="shared" ref="S4:S12" si="5">Q4/R4</f>
-        <v>83891449.052739367</v>
+        <v>89373772.63801004</v>
       </c>
       <c r="T4" s="5">
         <v>819200000</v>
       </c>
       <c r="U4" s="8">
-        <v>9.8420000000000005</v>
+        <v>9.0359999999999996</v>
       </c>
       <c r="V4" s="10">
         <f t="shared" ref="V4:V12" si="6">T4/U4</f>
-        <v>83235114.814062178</v>
+        <v>90659583.886675522</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -5017,31 +5017,31 @@
         <v>12800000</v>
       </c>
       <c r="O5" s="8">
-        <v>6.01</v>
+        <v>5.9989999999999997</v>
       </c>
       <c r="P5" s="10">
         <f t="shared" si="4"/>
-        <v>2129783.6938435943</v>
+        <v>2133688.9481580267</v>
       </c>
       <c r="Q5" s="5">
         <v>409600000</v>
       </c>
       <c r="R5" s="8">
-        <v>5.2789999999999999</v>
+        <v>5.1230000000000002</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" si="5"/>
-        <v>77590452.737260848</v>
+        <v>79953152.449736476</v>
       </c>
       <c r="T5" s="5">
         <v>409600000</v>
       </c>
       <c r="U5" s="8">
-        <v>5.0999999999999996</v>
+        <v>5.2809999999999997</v>
       </c>
       <c r="V5" s="10">
         <f t="shared" si="6"/>
-        <v>80313725.490196079</v>
+        <v>77561067.979549333</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -5092,31 +5092,31 @@
         <v>12800000</v>
       </c>
       <c r="O6" s="8">
-        <v>7.5590000000000002</v>
+        <v>7.6769999999999996</v>
       </c>
       <c r="P6" s="10">
         <f t="shared" si="4"/>
-        <v>1693345.6806455881</v>
+        <v>1667317.9627458644</v>
       </c>
       <c r="Q6" s="5">
         <v>409600000</v>
       </c>
       <c r="R6" s="8">
-        <v>6.2729999999999997</v>
+        <v>5.8109999999999999</v>
       </c>
       <c r="S6" s="10">
         <f t="shared" si="5"/>
-        <v>65295711.780647218</v>
+        <v>70487007.399759084</v>
       </c>
       <c r="T6" s="5">
         <v>409600000</v>
       </c>
       <c r="U6" s="8">
-        <v>6.2919999999999998</v>
+        <v>5.8890000000000002</v>
       </c>
       <c r="V6" s="10">
         <f t="shared" si="6"/>
-        <v>65098537.825810552</v>
+        <v>69553404.652742401</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -5167,31 +5167,31 @@
         <v>12800000</v>
       </c>
       <c r="O7" s="8">
-        <v>8.9529999999999994</v>
+        <v>9.0359999999999996</v>
       </c>
       <c r="P7" s="10">
         <f t="shared" si="4"/>
-        <v>1429688.3726125322</v>
+        <v>1416555.998229305</v>
       </c>
       <c r="Q7" s="5">
         <v>409600000</v>
       </c>
       <c r="R7" s="8">
-        <v>6.62</v>
+        <v>6.6139999999999999</v>
       </c>
       <c r="S7" s="10">
         <f t="shared" si="5"/>
-        <v>61873111.782477342</v>
+        <v>61929241.003931053</v>
       </c>
       <c r="T7" s="5">
         <v>409600000</v>
       </c>
       <c r="U7" s="8">
-        <v>6.55</v>
+        <v>6.5419999999999998</v>
       </c>
       <c r="V7" s="10">
         <f t="shared" si="6"/>
-        <v>62534351.145038173</v>
+        <v>62610822.378477529</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -5242,31 +5242,31 @@
         <v>6400000</v>
       </c>
       <c r="O8" s="8">
-        <v>5.3319999999999999</v>
+        <v>5.2539999999999996</v>
       </c>
       <c r="P8" s="10">
         <f t="shared" si="4"/>
-        <v>1200300.0750187547</v>
+        <v>1218119.5279786831</v>
       </c>
       <c r="Q8" s="5">
         <v>409600000</v>
       </c>
       <c r="R8" s="8">
-        <v>7.734</v>
+        <v>7.5640000000000001</v>
       </c>
       <c r="S8" s="10">
         <f t="shared" si="5"/>
-        <v>52960951.64209982</v>
+        <v>54151242.728714965</v>
       </c>
       <c r="T8" s="5">
         <v>409600000</v>
       </c>
       <c r="U8" s="8">
-        <v>8.157</v>
+        <v>7.649</v>
       </c>
       <c r="V8" s="10">
         <f t="shared" si="6"/>
-        <v>50214539.659188427</v>
+        <v>53549483.59262649</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -5317,31 +5317,31 @@
         <v>6400000</v>
       </c>
       <c r="O9" s="8">
-        <v>6.0090000000000003</v>
+        <v>5.8129999999999997</v>
       </c>
       <c r="P9" s="10">
         <f t="shared" si="4"/>
-        <v>1065069.0630720586</v>
+        <v>1100980.5608119732</v>
       </c>
       <c r="Q9" s="5">
         <v>409600000</v>
       </c>
       <c r="R9" s="8">
-        <v>8.5150000000000006</v>
+        <v>8.3260000000000005</v>
       </c>
       <c r="S9" s="10">
         <f t="shared" si="5"/>
-        <v>48103347.034644738</v>
+        <v>49195291.856834009</v>
       </c>
       <c r="T9" s="5">
         <v>409600000</v>
       </c>
       <c r="U9" s="8">
-        <v>8.4700000000000006</v>
+        <v>8.6289999999999996</v>
       </c>
       <c r="V9" s="10">
         <f t="shared" si="6"/>
-        <v>48358913.813459262</v>
+        <v>47467841.001274772</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -5392,31 +5392,31 @@
         <v>6400000</v>
       </c>
       <c r="O10" s="8">
-        <v>6.827</v>
+        <v>6.5860000000000003</v>
       </c>
       <c r="P10" s="10">
         <f t="shared" si="4"/>
-        <v>937454.2258678776</v>
+        <v>971758.27512906166</v>
       </c>
       <c r="Q10" s="5">
         <v>409600000</v>
       </c>
       <c r="R10" s="8">
-        <v>9.1880000000000006</v>
+        <v>9.5090000000000003</v>
       </c>
       <c r="S10" s="10">
         <f t="shared" si="5"/>
-        <v>44579886.808881149</v>
+        <v>43074981.596382372</v>
       </c>
       <c r="T10" s="5">
         <v>409600000</v>
       </c>
       <c r="U10" s="8">
-        <v>9.2449999999999992</v>
+        <v>9.4849999999999994</v>
       </c>
       <c r="V10" s="10">
         <f t="shared" si="6"/>
-        <v>44305029.745808549</v>
+        <v>43183974.696889825</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -5467,31 +5467,31 @@
         <v>6400000</v>
       </c>
       <c r="O11" s="8">
-        <v>7.4939999999999998</v>
+        <v>7.351</v>
       </c>
       <c r="P11" s="10">
         <f t="shared" si="4"/>
-        <v>854016.54657058988</v>
+        <v>870629.84627941775</v>
       </c>
       <c r="Q11" s="5">
         <v>204800000</v>
       </c>
       <c r="R11" s="8">
-        <v>5.1660000000000004</v>
+        <v>5.0060000000000002</v>
       </c>
       <c r="S11" s="10">
         <f t="shared" si="5"/>
-        <v>39643825.009678662</v>
+        <v>40910906.911705948</v>
       </c>
       <c r="T11" s="5">
         <v>204800000</v>
       </c>
       <c r="U11" s="8">
-        <v>5.1769999999999996</v>
+        <v>5.2359999999999998</v>
       </c>
       <c r="V11" s="10">
         <f t="shared" si="6"/>
-        <v>39559590.496426508</v>
+        <v>39113827.349121466</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -5542,31 +5542,31 @@
         <v>6400000</v>
       </c>
       <c r="O12" s="8">
-        <v>8.4009999999999998</v>
+        <v>8.2550000000000008</v>
       </c>
       <c r="P12" s="10">
         <f t="shared" si="4"/>
-        <v>761814.06975360075</v>
+        <v>775287.70442156261</v>
       </c>
       <c r="Q12" s="5">
         <v>204800000</v>
       </c>
       <c r="R12" s="8">
-        <v>5.4249999999999998</v>
+        <v>5.3250000000000002</v>
       </c>
       <c r="S12" s="10">
         <f t="shared" si="5"/>
-        <v>37751152.073732719</v>
+        <v>38460093.896713614</v>
       </c>
       <c r="T12" s="5">
         <v>204800000</v>
       </c>
       <c r="U12" s="8">
-        <v>5.4980000000000002</v>
+        <v>5.4669999999999996</v>
       </c>
       <c r="V12" s="10">
         <f t="shared" si="6"/>
-        <v>37249909.057839215</v>
+        <v>37461130.418876901</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -5653,31 +5653,31 @@
         <v>3200000</v>
       </c>
       <c r="O15" s="8">
-        <v>17.152000000000001</v>
+        <v>16.428999999999998</v>
       </c>
       <c r="P15" s="10">
         <f>N15/O15</f>
-        <v>186567.16417910447</v>
+        <v>194777.52754275978</v>
       </c>
       <c r="Q15" s="5">
-        <v>1638400000</v>
+        <v>3276800000</v>
       </c>
       <c r="R15" s="8">
-        <v>5.7009999999999996</v>
+        <v>9.3260000000000005</v>
       </c>
       <c r="S15" s="10">
         <f>Q15/R15</f>
-        <v>287388177.51271707</v>
+        <v>351361784.25906068</v>
       </c>
       <c r="T15" s="5">
         <v>3276800000</v>
       </c>
       <c r="U15" s="8">
-        <v>7.9290000000000003</v>
+        <v>7.6970000000000001</v>
       </c>
       <c r="V15" s="10">
         <f>T15/U15</f>
-        <v>413267751.29272288</v>
+        <v>425724308.17201507</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -5728,31 +5728,31 @@
         <v>3200000</v>
       </c>
       <c r="O16" s="8">
-        <v>28.861999999999998</v>
+        <v>27.652000000000001</v>
       </c>
       <c r="P16" s="10">
         <f t="shared" ref="P16:P24" si="11">N16/O16</f>
-        <v>110872.42741320768</v>
+        <v>115723.99826414003</v>
       </c>
       <c r="Q16" s="5">
         <v>409600000</v>
       </c>
       <c r="R16" s="8">
-        <v>6.0730000000000004</v>
+        <v>6.2990000000000004</v>
       </c>
       <c r="S16" s="10">
         <f t="shared" ref="S16:S24" si="12">Q16/R16</f>
-        <v>67446072.781162515</v>
+        <v>65026194.634068899</v>
       </c>
       <c r="T16" s="5">
         <v>1638400000</v>
       </c>
       <c r="U16" s="8">
-        <v>7.6619999999999999</v>
+        <v>7.4119999999999999</v>
       </c>
       <c r="V16" s="10">
         <f t="shared" ref="V16:V24" si="13">T16/U16</f>
-        <v>213834507.96136779</v>
+        <v>221046950.89044791</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -5803,31 +5803,31 @@
         <v>3200000</v>
       </c>
       <c r="O17" s="8">
-        <v>40.649000000000001</v>
+        <v>38.869999999999997</v>
       </c>
       <c r="P17" s="10">
         <f t="shared" si="11"/>
-        <v>78722.723806243695</v>
+        <v>82325.701054798046</v>
       </c>
       <c r="Q17" s="5">
         <v>204800000</v>
       </c>
       <c r="R17" s="8">
-        <v>5.282</v>
+        <v>5.4420000000000002</v>
       </c>
       <c r="S17" s="10">
         <f t="shared" si="12"/>
-        <v>38773191.972737603</v>
+        <v>37633223.079750091</v>
       </c>
       <c r="T17" s="5">
-        <v>819200000</v>
+        <v>1638400000</v>
       </c>
       <c r="U17" s="8">
-        <v>5.125</v>
+        <v>8.6519999999999992</v>
       </c>
       <c r="V17" s="10">
         <f t="shared" si="13"/>
-        <v>159843902.43902439</v>
+        <v>189366620.43458161</v>
       </c>
     </row>
     <row r="18" spans="1:22">
@@ -5878,31 +5878,31 @@
         <v>3200000</v>
       </c>
       <c r="O18" s="8">
-        <v>52.265000000000001</v>
+        <v>50.551000000000002</v>
       </c>
       <c r="P18" s="10">
         <f t="shared" si="11"/>
-        <v>61226.442169712042</v>
+        <v>63302.407469684076</v>
       </c>
       <c r="Q18" s="5">
         <v>204800000</v>
       </c>
       <c r="R18" s="8">
-        <v>7.6929999999999996</v>
+        <v>7.7519999999999998</v>
       </c>
       <c r="S18" s="10">
         <f t="shared" si="12"/>
-        <v>26621604.055634994</v>
+        <v>26418988.648090817</v>
       </c>
       <c r="T18" s="5">
         <v>819200000</v>
       </c>
       <c r="U18" s="8">
-        <v>6.085</v>
+        <v>5.9809999999999999</v>
       </c>
       <c r="V18" s="10">
         <f t="shared" si="13"/>
-        <v>134626129.82744452</v>
+        <v>136967062.36415315</v>
       </c>
     </row>
     <row r="19" spans="1:22">
@@ -5953,31 +5953,31 @@
         <v>3200000</v>
       </c>
       <c r="O19" s="8">
-        <v>63.898000000000003</v>
+        <v>61.862000000000002</v>
       </c>
       <c r="P19" s="10">
         <f t="shared" si="11"/>
-        <v>50079.814704685588</v>
+        <v>51728.039830590671</v>
       </c>
       <c r="Q19" s="5">
         <v>102400000</v>
       </c>
       <c r="R19" s="8">
-        <v>6.09</v>
+        <v>5.9269999999999996</v>
       </c>
       <c r="S19" s="10">
         <f t="shared" si="12"/>
-        <v>16814449.917898193</v>
+        <v>17276868.567572128</v>
       </c>
       <c r="T19" s="5">
         <v>409600000</v>
       </c>
       <c r="U19" s="8">
-        <v>7.5609999999999999</v>
+        <v>7.55</v>
       </c>
       <c r="V19" s="10">
         <f t="shared" si="13"/>
-        <v>54172728.475069433</v>
+        <v>54251655.629139073</v>
       </c>
     </row>
     <row r="20" spans="1:22">
@@ -6028,31 +6028,31 @@
         <v>3200000</v>
       </c>
       <c r="O20" s="8">
-        <v>74.462000000000003</v>
+        <v>73.462000000000003</v>
       </c>
       <c r="P20" s="10">
         <f t="shared" si="11"/>
-        <v>42974.940237973729</v>
+        <v>43559.935749094766</v>
       </c>
       <c r="Q20" s="5">
         <v>102400000</v>
       </c>
       <c r="R20" s="8">
-        <v>7.0529999999999999</v>
+        <v>6.5949999999999998</v>
       </c>
       <c r="S20" s="10">
         <f t="shared" si="12"/>
-        <v>14518644.548419112</v>
+        <v>15526914.32903715</v>
       </c>
       <c r="T20" s="5">
         <v>409600000</v>
       </c>
       <c r="U20" s="8">
-        <v>8.5419999999999998</v>
+        <v>8.1010000000000009</v>
       </c>
       <c r="V20" s="10">
         <f t="shared" si="13"/>
-        <v>47951299.461484432</v>
+        <v>50561659.054437719</v>
       </c>
     </row>
     <row r="21" spans="1:22">
@@ -6103,31 +6103,31 @@
         <v>3200000</v>
       </c>
       <c r="O21" s="8">
-        <v>85.436000000000007</v>
+        <v>84.179000000000002</v>
       </c>
       <c r="P21" s="10">
         <f t="shared" si="11"/>
-        <v>37454.937028887114</v>
+        <v>38014.231577946994</v>
       </c>
       <c r="Q21" s="5">
         <v>102400000</v>
       </c>
       <c r="R21" s="8">
-        <v>8.0419999999999998</v>
+        <v>7.883</v>
       </c>
       <c r="S21" s="10">
         <f t="shared" si="12"/>
-        <v>12733150.957473265</v>
+        <v>12989978.434606114</v>
       </c>
       <c r="T21" s="5">
         <v>409600000</v>
       </c>
       <c r="U21" s="8">
-        <v>9.8320000000000007</v>
+        <v>9.5730000000000004</v>
       </c>
       <c r="V21" s="10">
         <f t="shared" si="13"/>
-        <v>41659886.086248979</v>
+        <v>42787005.118562624</v>
       </c>
     </row>
     <row r="22" spans="1:22">
@@ -6178,31 +6178,31 @@
         <v>3200000</v>
       </c>
       <c r="O22" s="8">
-        <v>97.494</v>
+        <v>96.257000000000005</v>
       </c>
       <c r="P22" s="10">
         <f t="shared" si="11"/>
-        <v>32822.53266867705</v>
+        <v>33244.335476900378</v>
       </c>
       <c r="Q22" s="5">
-        <v>25600000</v>
+        <v>51200000</v>
       </c>
       <c r="R22" s="8">
-        <v>5.0270000000000001</v>
+        <v>9.6050000000000004</v>
       </c>
       <c r="S22" s="10">
         <f t="shared" si="12"/>
-        <v>5092500.4973145016</v>
+        <v>5330557.0015616864</v>
       </c>
       <c r="T22" s="5">
         <v>51200000</v>
       </c>
       <c r="U22" s="8">
-        <v>7.2030000000000003</v>
+        <v>7.3810000000000002</v>
       </c>
       <c r="V22" s="10">
         <f t="shared" si="13"/>
-        <v>7108149.3822018597</v>
+        <v>6936729.4404552225</v>
       </c>
     </row>
     <row r="23" spans="1:22">
@@ -6253,31 +6253,31 @@
         <v>3200000</v>
       </c>
       <c r="O23" s="8">
-        <v>111.529</v>
+        <v>107.12</v>
       </c>
       <c r="P23" s="10">
         <f t="shared" si="11"/>
-        <v>28692.089053071399</v>
+        <v>29873.039581777444</v>
       </c>
       <c r="Q23" s="5">
         <v>12800000</v>
       </c>
       <c r="R23" s="8">
-        <v>6.0579999999999998</v>
+        <v>6.0549999999999997</v>
       </c>
       <c r="S23" s="10">
         <f t="shared" si="12"/>
-        <v>2112908.550676791</v>
+        <v>2113955.4087530966</v>
       </c>
       <c r="T23" s="5">
         <v>12800000</v>
       </c>
       <c r="U23" s="8">
-        <v>5.84</v>
+        <v>6.12</v>
       </c>
       <c r="V23" s="10">
         <f t="shared" si="13"/>
-        <v>2191780.8219178081</v>
+        <v>2091503.2679738561</v>
       </c>
     </row>
     <row r="24" spans="1:22">
@@ -6328,31 +6328,31 @@
         <v>3200000</v>
       </c>
       <c r="O24" s="8">
-        <v>123.244</v>
+        <v>118.057</v>
       </c>
       <c r="P24" s="10">
         <f t="shared" si="11"/>
-        <v>25964.752848008829</v>
+        <v>27105.550708556035</v>
       </c>
       <c r="Q24" s="5">
         <v>12800000</v>
       </c>
       <c r="R24" s="8">
-        <v>7.2610000000000001</v>
+        <v>7.5369999999999999</v>
       </c>
       <c r="S24" s="10">
         <f t="shared" si="12"/>
-        <v>1762842.5836661616</v>
+        <v>1698288.4436778559</v>
       </c>
       <c r="T24" s="5">
         <v>12800000</v>
       </c>
       <c r="U24" s="8">
-        <v>7.2759999999999998</v>
+        <v>7.5839999999999996</v>
       </c>
       <c r="V24" s="10">
         <f t="shared" si="13"/>
-        <v>1759208.3562396921</v>
+        <v>1687763.7130801689</v>
       </c>
     </row>
     <row r="25" spans="1:22">
@@ -6438,31 +6438,31 @@
         <v>3200000</v>
       </c>
       <c r="O27" s="8">
-        <v>86.546999999999997</v>
+        <v>85.010999999999996</v>
       </c>
       <c r="P27" s="10">
         <f>N27/O27</f>
-        <v>36974.129663650965</v>
+        <v>37642.187481620029</v>
       </c>
       <c r="Q27" s="5">
         <v>102400000</v>
       </c>
       <c r="R27" s="8">
-        <v>6.665</v>
+        <v>6.2240000000000002</v>
       </c>
       <c r="S27" s="10">
         <f>Q27/R27</f>
-        <v>15363840.96024006</v>
+        <v>16452442.159383032</v>
       </c>
       <c r="T27" s="5">
         <v>409600000</v>
       </c>
       <c r="U27" s="8">
-        <v>7.9119999999999999</v>
+        <v>5.6589999999999998</v>
       </c>
       <c r="V27" s="10">
         <f>T27/U27</f>
-        <v>51769464.105156727</v>
+        <v>72380279.201272309</v>
       </c>
     </row>
     <row r="28" spans="1:22">
@@ -6513,31 +6513,31 @@
         <v>3200000</v>
       </c>
       <c r="O28" s="8">
-        <v>99.692999999999998</v>
+        <v>95.278999999999996</v>
       </c>
       <c r="P28" s="10">
         <f t="shared" ref="P28:P32" si="18">N28/O28</f>
-        <v>32098.54252555345</v>
+        <v>33585.57499553942</v>
       </c>
       <c r="Q28" s="5">
         <v>102400000</v>
       </c>
       <c r="R28" s="8">
-        <v>6.3220000000000001</v>
+        <v>6.9470000000000001</v>
       </c>
       <c r="S28" s="10">
         <f t="shared" ref="S28:S32" si="19">Q28/R28</f>
-        <v>16197405.884213855</v>
+        <v>14740175.615373543</v>
       </c>
       <c r="T28" s="5">
         <v>409600000</v>
       </c>
       <c r="U28" s="8">
-        <v>9.26</v>
+        <v>7.06</v>
       </c>
       <c r="V28" s="10">
         <f t="shared" ref="V28:V32" si="20">T28/U28</f>
-        <v>44233261.339092873</v>
+        <v>58016997.167138815</v>
       </c>
     </row>
     <row r="29" spans="1:22">
@@ -6588,31 +6588,31 @@
         <v>3200000</v>
       </c>
       <c r="O29" s="8">
-        <v>108.77500000000001</v>
+        <v>105.724</v>
       </c>
       <c r="P29" s="10">
         <f t="shared" si="18"/>
-        <v>29418.524477131694</v>
+        <v>30267.488933449356</v>
       </c>
       <c r="Q29" s="5">
-        <v>102400000</v>
+        <v>51200000</v>
       </c>
       <c r="R29" s="8">
-        <v>9.6969999999999992</v>
+        <v>5.0709999999999997</v>
       </c>
       <c r="S29" s="10">
         <f t="shared" si="19"/>
-        <v>10559967.000103125</v>
+        <v>10096627.88404654</v>
       </c>
       <c r="T29" s="5">
         <v>102400000</v>
       </c>
       <c r="U29" s="8">
-        <v>6.6740000000000004</v>
+        <v>6.4649999999999999</v>
       </c>
       <c r="V29" s="10">
         <f t="shared" si="20"/>
-        <v>15343122.565178303</v>
+        <v>15839133.797370456</v>
       </c>
     </row>
     <row r="30" spans="1:22">
@@ -6663,31 +6663,31 @@
         <v>3200000</v>
       </c>
       <c r="O30" s="8">
-        <v>118.691</v>
+        <v>117.69799999999999</v>
       </c>
       <c r="P30" s="10">
         <f t="shared" si="18"/>
-        <v>26960.763663630772</v>
+        <v>27188.227497493586</v>
       </c>
       <c r="Q30" s="5">
         <v>51200000</v>
       </c>
       <c r="R30" s="8">
-        <v>6.6459999999999999</v>
+        <v>7.0979999999999999</v>
       </c>
       <c r="S30" s="10">
         <f t="shared" si="19"/>
-        <v>7703882.0343063502</v>
+        <v>7213299.5209918292</v>
       </c>
       <c r="T30" s="5">
-        <v>51200000</v>
+        <v>102400000</v>
       </c>
       <c r="U30" s="8">
-        <v>5.1449999999999996</v>
+        <v>10.243</v>
       </c>
       <c r="V30" s="10">
         <f t="shared" si="20"/>
-        <v>9951409.1350826062</v>
+        <v>9997071.1705555003</v>
       </c>
     </row>
     <row r="31" spans="1:22">
@@ -6738,31 +6738,31 @@
         <v>3200000</v>
       </c>
       <c r="O31" s="8">
-        <v>130.46299999999999</v>
+        <v>127.82</v>
       </c>
       <c r="P31" s="10">
         <f t="shared" si="18"/>
-        <v>24528.027103469951</v>
+        <v>25035.205758097327</v>
       </c>
       <c r="Q31" s="5">
         <v>51200000</v>
       </c>
       <c r="R31" s="8">
-        <v>8.6349999999999998</v>
+        <v>8.9440000000000008</v>
       </c>
       <c r="S31" s="10">
         <f t="shared" si="19"/>
-        <v>5929357.2669368852</v>
+        <v>5724508.050089445</v>
       </c>
       <c r="T31" s="5">
         <v>51200000</v>
       </c>
       <c r="U31" s="8">
-        <v>6.819</v>
+        <v>6.8550000000000004</v>
       </c>
       <c r="V31" s="10">
         <f t="shared" si="20"/>
-        <v>7508432.3214547588</v>
+        <v>7469000.7293946017</v>
       </c>
     </row>
     <row r="32" spans="1:22">
@@ -6813,31 +6813,31 @@
         <v>3200000</v>
       </c>
       <c r="O32" s="5">
-        <v>139.91399999999999</v>
+        <v>138.018</v>
       </c>
       <c r="P32" s="10">
         <f t="shared" si="18"/>
-        <v>22871.192303843793</v>
+        <v>23185.381616890551</v>
       </c>
       <c r="Q32" s="5">
         <v>25600000</v>
       </c>
       <c r="R32" s="8">
-        <v>5.4560000000000004</v>
+        <v>5.1539999999999999</v>
       </c>
       <c r="S32" s="10">
         <f t="shared" si="19"/>
-        <v>4692082.11143695</v>
+        <v>4967015.9099728363</v>
       </c>
       <c r="T32" s="5">
         <v>51200000</v>
       </c>
       <c r="U32" s="8">
-        <v>8.7550000000000008</v>
+        <v>8.75</v>
       </c>
       <c r="V32" s="10">
         <f t="shared" si="20"/>
-        <v>5848086.8075385485</v>
+        <v>5851428.5714285718</v>
       </c>
     </row>
   </sheetData>
@@ -6864,7 +6864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -6926,15 +6926,15 @@
       </c>
       <c r="F2" s="4">
         <f>Bench1!P15/Bench1!P3</f>
-        <v>3.9091651119402986E-2</v>
+        <v>4.2014121370746858E-2</v>
       </c>
       <c r="G2" s="4">
         <f>Bench1!S15/Bench1!S3</f>
-        <v>3.0089457989826345</v>
+        <v>3.4733004503538494</v>
       </c>
       <c r="H2" s="4">
         <f>Bench1!V15/Bench1!V3</f>
-        <v>4.4484802623281618</v>
+        <v>4.4173054436793562</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="2"/>
@@ -6961,15 +6961,15 @@
       </c>
       <c r="F3" s="4">
         <f>Bench1!P16/Bench1!P4</f>
-        <v>3.931207123553461E-2</v>
+        <v>4.1100101258498487E-2</v>
       </c>
       <c r="G3" s="4">
         <f>Bench1!S16/Bench1!S4</f>
-        <v>0.80396838465338383</v>
+        <v>0.72757580568344182</v>
       </c>
       <c r="H3" s="4">
         <f>Bench1!V16/Bench1!V4</f>
-        <v>2.5690420255807882</v>
+        <v>2.4382083108472745</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="2"/>
@@ -6996,15 +6996,15 @@
       </c>
       <c r="F4" s="4">
         <f>Bench1!P17/Bench1!P5</f>
-        <v>3.6962778912150357E-2</v>
+        <v>3.8583740674041675E-2</v>
       </c>
       <c r="G4" s="4">
         <f>Bench1!S17/Bench1!S5</f>
-        <v>0.49971601666035592</v>
+        <v>0.47069092245497979</v>
       </c>
       <c r="H4" s="4">
         <f>Bench1!V17/Bench1!V5</f>
-        <v>1.9902439024390244</v>
+        <v>2.4415164123901989</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
@@ -7031,15 +7031,15 @@
       </c>
       <c r="F5" s="4">
         <f>Bench1!P18/Bench1!P6</f>
-        <v>3.6157084090691662E-2</v>
+        <v>3.7966607980059734E-2</v>
       </c>
       <c r="G5" s="4">
         <f>Bench1!S18/Bench1!S6</f>
-        <v>0.40770830625243731</v>
+        <v>0.37480650154798761</v>
       </c>
       <c r="H5" s="4">
         <f>Bench1!V18/Bench1!V6</f>
-        <v>2.0680361544782251</v>
+        <v>1.9692359137268014</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
@@ -7066,15 +7066,15 @@
       </c>
       <c r="F6" s="4">
         <f>Bench1!P19/Bench1!P7</f>
-        <v>3.5028482894613286E-2</v>
+        <v>3.6516763117907601E-2</v>
       </c>
       <c r="G6" s="4">
         <f>Bench1!S19/Bench1!S7</f>
-        <v>0.27175697865353038</v>
+        <v>0.27897756031719251</v>
       </c>
       <c r="H6" s="4">
         <f>Bench1!V19/Bench1!V7</f>
-        <v>0.86628752810474796</v>
+        <v>0.86649006622516556</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="2"/>
@@ -7101,15 +7101,15 @@
       </c>
       <c r="F7" s="4">
         <f>Bench1!P20/Bench1!P8</f>
-        <v>3.5803497085761866E-2</v>
+        <v>3.5759984754022478E-2</v>
       </c>
       <c r="G7" s="4">
         <f>Bench1!S20/Bench1!S8</f>
-        <v>0.27413866439812845</v>
+        <v>0.28673237300985599</v>
       </c>
       <c r="H7" s="4">
         <f>Bench1!V20/Bench1!V8</f>
-        <v>0.95492858815265746</v>
+        <v>0.94420441920750509</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
@@ -7136,15 +7136,15 @@
       </c>
       <c r="F8" s="4">
         <f>Bench1!P21/Bench1!P9</f>
-        <v>3.5166674469778544E-2</v>
+        <v>3.4527613775407168E-2</v>
       </c>
       <c r="G8" s="4">
         <f>Bench1!S21/Bench1!S9</f>
-        <v>0.26470405371798061</v>
+        <v>0.26404921984016239</v>
       </c>
       <c r="H8" s="4">
         <f>Bench1!V21/Bench1!V9</f>
-        <v>0.86147274206672098</v>
+        <v>0.90138932414081263</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
@@ -7171,15 +7171,15 @@
       </c>
       <c r="F9" s="4">
         <f>Bench1!P22/Bench1!P10</f>
-        <v>3.5012411020165342E-2</v>
+        <v>3.4210498976697798E-2</v>
       </c>
       <c r="G9" s="4">
         <f>Bench1!S22/Bench1!S10</f>
-        <v>0.11423314103839267</v>
+        <v>0.12375065070275898</v>
       </c>
       <c r="H9" s="4">
         <f>Bench1!V22/Bench1!V10</f>
-        <v>0.16043662362904343</v>
+        <v>0.16063202818046335</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
@@ -7206,15 +7206,15 @@
       </c>
       <c r="F10" s="4">
         <f>Bench1!P23/Bench1!P11</f>
-        <v>3.359664302558079E-2</v>
+        <v>3.431198655713219E-2</v>
       </c>
       <c r="G10" s="4">
         <f>Bench1!S23/Bench1!S11</f>
-        <v>5.3297292835919455E-2</v>
+        <v>5.1672171758876964E-2</v>
       </c>
       <c r="H10" s="4">
         <f>Bench1!V23/Bench1!V11</f>
-        <v>5.5404537671232865E-2</v>
+        <v>5.347222222222222E-2</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="2"/>
@@ -7241,15 +7241,15 @@
       </c>
       <c r="F11" s="4">
         <f>Bench1!P24/Bench1!P12</f>
-        <v>3.408279510564409E-2</v>
+        <v>3.4961925171739079E-2</v>
       </c>
       <c r="G11" s="4">
         <f>Bench1!S24/Bench1!S12</f>
-        <v>4.6696391681586555E-2</v>
+        <v>4.4157158020432533E-2</v>
       </c>
       <c r="H11" s="4">
         <f>Bench1!V24/Bench1!V12</f>
-        <v>4.7227185266630015E-2</v>
+        <v>4.5053731540084387E-2</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
@@ -7361,15 +7361,15 @@
       </c>
       <c r="F3" s="4">
         <f>Bench1!P28/Bench1!P$27</f>
-        <v>0.86813517498721071</v>
+        <v>0.89223228623306294</v>
       </c>
       <c r="G3" s="4">
         <f>Bench1!S28/Bench1!S$27</f>
-        <v>1.0542549826004428</v>
+        <v>0.89592629912192323</v>
       </c>
       <c r="H3" s="4">
         <f>Bench1!V28/Bench1!V$27</f>
-        <v>0.85442764578833685</v>
+        <v>0.80155807365439102</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="19">
@@ -7394,15 +7394,15 @@
       </c>
       <c r="F4" s="4">
         <f>Bench1!P29/Bench1!P$27</f>
-        <v>0.79565157435072398</v>
+        <v>0.80408421928795715</v>
       </c>
       <c r="G4" s="4">
         <f>Bench1!S29/Bench1!S$27</f>
-        <v>0.6873259771063216</v>
+        <v>0.61368566357720378</v>
       </c>
       <c r="H4" s="4">
         <f>Bench1!V29/Bench1!V$27</f>
-        <v>0.29637398861252617</v>
+        <v>0.2188321732405259</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="19">
@@ -7427,15 +7427,15 @@
       </c>
       <c r="F5" s="4">
         <f>Bench1!P30/Bench1!P$27</f>
-        <v>0.72917912899882886</v>
+        <v>0.72228075243419598</v>
       </c>
       <c r="G5" s="4">
         <f>Bench1!S30/Bench1!S$27</f>
-        <v>0.50142943123683426</v>
+        <v>0.43843336151028467</v>
       </c>
       <c r="H5" s="4">
         <f>Bench1!V30/Bench1!V$27</f>
-        <v>0.19222546161321674</v>
+        <v>0.13811871522015035</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19">
@@ -7460,15 +7460,15 @@
       </c>
       <c r="F6" s="4">
         <f>Bench1!P31/Bench1!P$27</f>
-        <v>0.66338348803875435</v>
+        <v>0.6650837114692536</v>
       </c>
       <c r="G6" s="4">
         <f>Bench1!S31/Bench1!S$27</f>
-        <v>0.38592935726693689</v>
+        <v>0.34794275491949911</v>
       </c>
       <c r="H6" s="4">
         <f>Bench1!V31/Bench1!V$27</f>
-        <v>0.1450359290218507</v>
+        <v>0.10319110138584973</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19">
@@ -7493,15 +7493,15 @@
       </c>
       <c r="F7" s="4">
         <f>Bench1!P32/Bench1!P$27</f>
-        <v>0.61857283760024018</v>
+        <v>0.61594139894796329</v>
       </c>
       <c r="G7" s="4">
         <f>Bench1!S32/Bench1!S$27</f>
-        <v>0.30539772727272724</v>
+        <v>0.30190143577803646</v>
       </c>
       <c r="H7" s="4">
         <f>Bench1!V32/Bench1!V$27</f>
-        <v>0.11296402055968016</v>
+        <v>8.0842857142857147E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="19">

</xml_diff>